<commit_message>
Data: Estructura de los datos para el EDA
</commit_message>
<xml_diff>
--- a/data/eda_matrix.xlsx
+++ b/data/eda_matrix.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Source\Repos\DS4All_2020_Team28_Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{666D0A68-DD26-4223-80ED-7D8DB99AD3BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CBDED1-E04C-4797-BBDB-5BF002F9FE60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1EC1EFBC-92A0-4706-A539-7634088136E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="detalle" sheetId="1" r:id="rId1"/>
     <sheet name="deforestacion" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>

</xml_diff>

<commit_message>
Data: - Formato matrix de datos - Matrix de datos del IDEAM por cuenca y año-mes
</commit_message>
<xml_diff>
--- a/data/eda_matrix.xlsx
+++ b/data/eda_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Source\Repos\DS4All_2020_Team28_Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CBDED1-E04C-4797-BBDB-5BF002F9FE60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9305D142-3838-4DD2-85D2-5D4A682DCD50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1EC1EFBC-92A0-4706-A539-7634088136E3}"/>
   </bookViews>
@@ -475,20 +475,22 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="11.42578125" style="1"/>
-    <col min="7" max="7" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="1"/>
-    <col min="13" max="16" width="11.42578125" style="2"/>
-    <col min="17" max="17" width="11.42578125" style="3"/>
+    <col min="1" max="3" width="11.42578125" style="1"/>
+    <col min="4" max="5" width="11.42578125" style="2"/>
+    <col min="7" max="9" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="1"/>
+    <col min="16" max="17" width="11.42578125" style="2"/>
+    <col min="18" max="18" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -501,54 +503,54 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>